<commit_message>
feat: make exports german for logbook
</commit_message>
<xml_diff>
--- a/templates/export/logbook.xlsx
+++ b/templates/export/logbook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/d050092/git/private/Socratec/traccar/templates/export/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F035C2C5-8894-4F45-AE16-8227AF17FF0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFECB956-992A-0D49-9F75-5ED4E41730F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="680" windowWidth="34560" windowHeight="20180" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -87,66 +87,21 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
-    <t>Report type:</t>
-  </si>
-  <si>
-    <t>Logbook</t>
-  </si>
-  <si>
     <t>Device:</t>
   </si>
   <si>
     <t>${device.deviceName}</t>
   </si>
   <si>
-    <t>Group:</t>
-  </si>
-  <si>
     <t>${device.groupName}</t>
   </si>
   <si>
-    <t>Period:</t>
-  </si>
-  <si>
     <t>${dateTool.format("YYYY-MM-dd HH:mm:ss", from, locale, timezone)+" - "+dateTool.format("YYYY-MM-dd HH:mm:ss", to, locale, timezone)}</t>
   </si>
   <si>
     <t>Start</t>
   </si>
   <si>
-    <t>Start Address</t>
-  </si>
-  <si>
-    <t>Start Odometer</t>
-  </si>
-  <si>
-    <t>End</t>
-  </si>
-  <si>
-    <t>End Address</t>
-  </si>
-  <si>
-    <t>End Odometer</t>
-  </si>
-  <si>
-    <t>Duration</t>
-  </si>
-  <si>
-    <t>Length</t>
-  </si>
-  <si>
-    <t>Top speed</t>
-  </si>
-  <si>
-    <t>Average speed</t>
-  </si>
-  <si>
-    <t>Spent Fuel</t>
-  </si>
-  <si>
-    <t>Driver</t>
-  </si>
-  <si>
     <t>${dateTool.format("YYYY-MM-dd HH:mm:ss", entry.startTime, locale, timezone)}</t>
   </si>
   <si>
@@ -183,42 +138,15 @@
     <t>${entry.driverId}</t>
   </si>
   <si>
-    <t>Type</t>
-  </si>
-  <si>
     <t>${entry.type.value == 1 ? "Business" : entry.type.value == 2 ? "Private" : "None"}</t>
   </si>
   <si>
-    <t>Note</t>
-  </si>
-  <si>
     <t>${entry.notes}</t>
   </si>
   <si>
     <t>${device.objects.size()}</t>
   </si>
   <si>
-    <t>Entries:</t>
-  </si>
-  <si>
-    <t>Distance total:</t>
-  </si>
-  <si>
-    <t>Distance private</t>
-  </si>
-  <si>
-    <t>Distance business</t>
-  </si>
-  <si>
-    <t>Duration total</t>
-  </si>
-  <si>
-    <t>Duration private</t>
-  </si>
-  <si>
-    <t>Duration business</t>
-  </si>
-  <si>
     <t>${distanceUnit.equals("mi") ? "".format("%.1f mi", device.totalDistance * 0.000621371) : distanceUnit.equals("nmi") ? "".format("%.1f nmi", device.totalDistance * 0.000539957) : "".format("%.1f km", device.totalDistance * 0.001)}</t>
   </si>
   <si>
@@ -235,6 +163,78 @@
   </si>
   <si>
     <t>${device.businessDuration/86400000.0}</t>
+  </si>
+  <si>
+    <t>Start Adresse</t>
+  </si>
+  <si>
+    <t>Ende</t>
+  </si>
+  <si>
+    <t>Kilometerstand Ende</t>
+  </si>
+  <si>
+    <t>Kilometerstand Start</t>
+  </si>
+  <si>
+    <t>Ende Adresse</t>
+  </si>
+  <si>
+    <t>Dauer</t>
+  </si>
+  <si>
+    <t>Distanz</t>
+  </si>
+  <si>
+    <t>Höchstgeschwindigkeit</t>
+  </si>
+  <si>
+    <t>Durchschnittsgeschwindigkeit</t>
+  </si>
+  <si>
+    <t>Kraftstoffverbrauch</t>
+  </si>
+  <si>
+    <t>Fahrer</t>
+  </si>
+  <si>
+    <t>Typ</t>
+  </si>
+  <si>
+    <t>Notiz</t>
+  </si>
+  <si>
+    <t>Report Typ:</t>
+  </si>
+  <si>
+    <t>Fahrtenbuch</t>
+  </si>
+  <si>
+    <t>Gruppe</t>
+  </si>
+  <si>
+    <t>Periode:</t>
+  </si>
+  <si>
+    <t>Einträge:</t>
+  </si>
+  <si>
+    <t>Distanz total:</t>
+  </si>
+  <si>
+    <t>Distanz privat</t>
+  </si>
+  <si>
+    <t>Distanz geschäftlich</t>
+  </si>
+  <si>
+    <t>Dauer geschäftlich</t>
+  </si>
+  <si>
+    <t>Dauer privat</t>
+  </si>
+  <si>
+    <t>Dauer total</t>
   </si>
 </sst>
 </file>
@@ -850,7 +850,7 @@
   <dimension ref="A1:N1004"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -886,10 +886,10 @@
     </row>
     <row r="2" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>0</v>
+        <v>39</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>1</v>
+        <v>40</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -916,10 +916,10 @@
     </row>
     <row r="4" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
@@ -933,10 +933,10 @@
     </row>
     <row r="5" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>4</v>
+        <v>41</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -950,10 +950,10 @@
     </row>
     <row r="6" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>6</v>
+        <v>42</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -967,10 +967,10 @@
     </row>
     <row r="7" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="7"/>
@@ -984,17 +984,17 @@
     </row>
     <row r="8" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>44</v>
+        <v>20</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>47</v>
+        <v>23</v>
       </c>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
@@ -1005,17 +1005,17 @@
     </row>
     <row r="9" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>45</v>
+        <v>21</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>48</v>
+        <v>24</v>
       </c>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
@@ -1026,17 +1026,17 @@
     </row>
     <row r="10" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>49</v>
+        <v>25</v>
       </c>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
@@ -1060,90 +1060,90 @@
     </row>
     <row r="12" spans="1:14" s="10" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="9" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="H12" s="9" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="I12" s="9" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="J12" s="9" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="K12" s="9" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="L12" s="9" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="M12" s="9" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="N12" s="9" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:14" s="16" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="11" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="F13" s="13" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="G13" s="14" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="H13" s="13" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="I13" s="15" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="J13" s="15" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="K13" s="15" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="L13" s="15" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="M13" s="15" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="N13" s="15" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
     </row>
     <row r="25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
feat: enable geofence export for PDf and excel
</commit_message>
<xml_diff>
--- a/templates/export/logbook.xlsx
+++ b/templates/export/logbook.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11102"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10110"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/d050092/git/private/Socratec/traccar/templates/export/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFECB956-992A-0D49-9F75-5ED4E41730F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A85B5308-6C1E-E346-ACBE-98E52B522DED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="680" windowWidth="34560" windowHeight="20180" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -50,7 +50,7 @@
             <rFont val="Arial"/>
             <family val="2"/>
           </rPr>
-          <t>jx:area(lastCell="N13")</t>
+          <t>jx:area(lastCell="P13")</t>
         </r>
       </text>
     </comment>
@@ -63,7 +63,7 @@
             <rFont val="Arial"/>
             <family val="2"/>
           </rPr>
-          <t>jx:each(items="devices", var="device", lastCell="N13" multisheet="sheetNames")</t>
+          <t>jx:each(items="devices", var="device", lastCell="P13" multisheet="sheetNames")</t>
         </r>
       </text>
     </comment>
@@ -76,7 +76,7 @@
             <rFont val="Arial"/>
             <family val="2"/>
           </rPr>
-          <t>jx:each(items="device.objects", var="entry", lastCell="N13")</t>
+          <t>jx:each(items="device.objects", var="entry", lastCell="P13")</t>
         </r>
       </text>
     </comment>
@@ -85,7 +85,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <si>
     <t>Device:</t>
   </si>
@@ -235,6 +235,18 @@
   </si>
   <si>
     <t>Dauer total</t>
+  </si>
+  <si>
+    <t>Start Geofence</t>
+  </si>
+  <si>
+    <t>${entry.startGeofences}</t>
+  </si>
+  <si>
+    <t>Ende Geofences</t>
+  </si>
+  <si>
+    <t>${entry.endGeofences}</t>
   </si>
 </sst>
 </file>
@@ -847,10 +859,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N1004"/>
+  <dimension ref="A1:P1004"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -867,11 +879,11 @@
     <col min="10" max="10" width="16" customWidth="1"/>
     <col min="11" max="11" width="14.5" customWidth="1"/>
     <col min="12" max="12" width="17.5" customWidth="1"/>
-    <col min="13" max="28" width="8.6640625" customWidth="1"/>
-    <col min="29" max="1025" width="14.1640625" customWidth="1"/>
+    <col min="13" max="30" width="8.6640625" customWidth="1"/>
+    <col min="31" max="1027" width="14.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
@@ -884,7 +896,7 @@
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>
     </row>
-    <row r="2" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>39</v>
       </c>
@@ -901,7 +913,7 @@
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
       <c r="B3" s="6"/>
       <c r="C3" s="3"/>
@@ -914,7 +926,7 @@
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
     </row>
-    <row r="4" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>0</v>
       </c>
@@ -931,7 +943,7 @@
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
     </row>
-    <row r="5" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>41</v>
       </c>
@@ -948,7 +960,7 @@
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
     </row>
-    <row r="6" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>42</v>
       </c>
@@ -965,7 +977,7 @@
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
     </row>
-    <row r="7" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>43</v>
       </c>
@@ -982,7 +994,7 @@
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
     </row>
-    <row r="8" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>44</v>
       </c>
@@ -1003,7 +1015,7 @@
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
     </row>
-    <row r="9" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>45</v>
       </c>
@@ -1024,7 +1036,7 @@
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
     </row>
-    <row r="10" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>46</v>
       </c>
@@ -1045,7 +1057,7 @@
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" s="3"/>
       <c r="B11" s="8"/>
       <c r="C11" s="3"/>
@@ -1058,7 +1070,7 @@
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
     </row>
-    <row r="12" spans="1:14" s="10" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" s="10" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="9" t="s">
         <v>4</v>
       </c>
@@ -1099,10 +1111,16 @@
         <v>37</v>
       </c>
       <c r="N12" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="O12" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="P12" s="9" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:14" s="16" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" s="16" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="11" t="s">
         <v>5</v>
       </c>
@@ -1143,6 +1161,12 @@
         <v>17</v>
       </c>
       <c r="N13" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="O13" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="P13" s="15" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>